<commit_message>
Update .DS_Store and bsale-octaba-entrega.xlsx files
</commit_message>
<xml_diff>
--- a/data/bsale/bsale-octaba-entrega.xlsx
+++ b/data/bsale/bsale-octaba-entrega.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/data/bsale/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2D4E8C-BD66-6D46-BC59-6098EE02AA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235C6018-C76F-B647-85F5-AF1FA4174AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -308,7 +308,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -670,7 +680,7 @@
   <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K16"/>
+      <selection activeCell="T16" sqref="A1:T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -800,9 +810,6 @@
       <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="O2">
-        <v>14</v>
-      </c>
       <c r="Q2">
         <v>100</v>
       </c>
@@ -859,9 +866,6 @@
       <c r="N3" t="s">
         <v>24</v>
       </c>
-      <c r="O3">
-        <v>40</v>
-      </c>
       <c r="Q3">
         <v>100</v>
       </c>
@@ -918,9 +922,6 @@
       <c r="N4" t="s">
         <v>24</v>
       </c>
-      <c r="O4">
-        <v>40</v>
-      </c>
       <c r="Q4">
         <v>100</v>
       </c>
@@ -977,9 +978,6 @@
       <c r="N5" t="s">
         <v>24</v>
       </c>
-      <c r="O5">
-        <v>28</v>
-      </c>
       <c r="Q5">
         <v>100</v>
       </c>
@@ -1036,9 +1034,6 @@
       <c r="N6" t="s">
         <v>24</v>
       </c>
-      <c r="O6">
-        <v>14</v>
-      </c>
       <c r="Q6">
         <v>100</v>
       </c>
@@ -1095,9 +1090,6 @@
       <c r="N7" t="s">
         <v>24</v>
       </c>
-      <c r="O7">
-        <v>14</v>
-      </c>
       <c r="Q7">
         <v>100</v>
       </c>
@@ -1154,9 +1146,6 @@
       <c r="N8" t="s">
         <v>24</v>
       </c>
-      <c r="O8">
-        <v>40</v>
-      </c>
       <c r="Q8">
         <v>100</v>
       </c>
@@ -1213,9 +1202,6 @@
       <c r="N9" t="s">
         <v>24</v>
       </c>
-      <c r="O9">
-        <v>40</v>
-      </c>
       <c r="Q9">
         <v>100</v>
       </c>
@@ -1272,9 +1258,6 @@
       <c r="N10" t="s">
         <v>24</v>
       </c>
-      <c r="O10">
-        <v>28</v>
-      </c>
       <c r="Q10">
         <v>100</v>
       </c>
@@ -1331,9 +1314,6 @@
       <c r="N11" t="s">
         <v>24</v>
       </c>
-      <c r="O11">
-        <v>14</v>
-      </c>
       <c r="Q11">
         <v>100</v>
       </c>
@@ -1390,9 +1370,6 @@
       <c r="N12" t="s">
         <v>24</v>
       </c>
-      <c r="O12">
-        <v>14</v>
-      </c>
       <c r="Q12">
         <v>100</v>
       </c>
@@ -1449,9 +1426,6 @@
       <c r="N13" t="s">
         <v>24</v>
       </c>
-      <c r="O13">
-        <v>40</v>
-      </c>
       <c r="Q13">
         <v>100</v>
       </c>
@@ -1508,9 +1482,6 @@
       <c r="N14" t="s">
         <v>24</v>
       </c>
-      <c r="O14">
-        <v>40</v>
-      </c>
       <c r="Q14">
         <v>100</v>
       </c>
@@ -1567,9 +1538,6 @@
       <c r="N15" t="s">
         <v>24</v>
       </c>
-      <c r="O15">
-        <v>28</v>
-      </c>
       <c r="Q15">
         <v>100</v>
       </c>
@@ -1626,9 +1594,6 @@
       <c r="N16" t="s">
         <v>24</v>
       </c>
-      <c r="O16">
-        <v>14</v>
-      </c>
       <c r="Q16">
         <v>100</v>
       </c>
@@ -1643,23 +1608,24 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L2:L35">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  <conditionalFormatting sqref="J2:J16">
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L36">
+  <conditionalFormatting sqref="K2:K16">
     <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M36">
+  <conditionalFormatting sqref="L17:L35 K2:K16">
     <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K16">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="L17:L36 K2:K16">
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K16">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="M17:M36 L2:L16">
+    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L16">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>